<commit_message>
maps on mouse catching data
</commit_message>
<xml_diff>
--- a/Data/Field_tracking_data/Rodents_catching_data.xlsx
+++ b/Data/Field_tracking_data/Rodents_catching_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f06612572c8e6b/Documents/GitHub/Namibia_project/Data/Field_tracking_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{BB9031C0-2030-4706-B07B-FEFB07EC1D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{415ED5D1-E9C0-4570-8365-7BF86134F517}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="8_{BB9031C0-2030-4706-B07B-FEFB07EC1D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61F97EA1-6C46-4AB3-ACBE-A341F31E1579}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{181B5E23-3E4F-4106-9299-8C1243943CD4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="93">
   <si>
     <t>R01</t>
   </si>
@@ -86,9 +86,6 @@
     <t>R16</t>
   </si>
   <si>
-    <t>R17</t>
-  </si>
-  <si>
     <t>R18</t>
   </si>
   <si>
@@ -299,7 +296,25 @@
     <t>Sample_ID</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Vole?</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Elephantulus_intufi</t>
+  </si>
+  <si>
+    <t>House_mouse?</t>
+  </si>
+  <si>
+    <t>Thallomys_paedulcus</t>
+  </si>
+  <si>
+    <t>House_outdoors</t>
+  </si>
+  <si>
+    <t>Farm</t>
   </si>
 </sst>
 </file>
@@ -668,7 +683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84E11E3-459E-46DA-95D2-AC4A7DA608C0}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -683,39 +698,36 @@
     <col min="8" max="8" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -726,25 +738,25 @@
         <v>18.189302000000001</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G2">
         <v>38.700000000000003</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -755,25 +767,25 @@
         <v>18.189302000000001</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3">
         <v>43.5</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -784,25 +796,25 @@
         <v>18.190221999999999</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4">
         <v>32.5</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -813,25 +825,25 @@
         <v>18.187052999999999</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -842,25 +854,25 @@
         <v>18.187052999999999</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6">
         <v>43.5</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -871,25 +883,25 @@
         <v>18.187052999999999</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7">
         <v>84.16</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -900,25 +912,25 @@
         <v>18.187052999999999</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G8">
         <v>45.5</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -929,25 +941,25 @@
         <v>18.187052999999999</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9">
         <v>46.8</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -957,11 +969,26 @@
       <c r="C10">
         <v>18.192715</v>
       </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10">
+        <v>116</v>
+      </c>
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
       <c r="I10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -971,11 +998,26 @@
       <c r="C11">
         <v>18.192674</v>
       </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>91</v>
+      </c>
       <c r="I11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -985,11 +1027,26 @@
       <c r="C12">
         <v>18.192674</v>
       </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12">
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
+        <v>91</v>
+      </c>
       <c r="I12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -999,11 +1056,26 @@
       <c r="C13">
         <v>18.192674</v>
       </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
       <c r="I13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1013,11 +1085,26 @@
       <c r="C14">
         <v>18.192674</v>
       </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
+        <v>91</v>
+      </c>
       <c r="I14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1027,11 +1114,23 @@
       <c r="C15">
         <v>18.192468999999999</v>
       </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>91</v>
+      </c>
       <c r="I15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1041,8 +1140,23 @@
       <c r="C16">
         <v>18.192468999999999</v>
       </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1055,8 +1169,23 @@
       <c r="C17">
         <v>18.192468999999999</v>
       </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
+        <v>91</v>
+      </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1064,13 +1193,28 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-22.613507999999999</v>
+        <v>-22.615736999999999</v>
       </c>
       <c r="C18">
-        <v>18.192468999999999</v>
+        <v>18.192335</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
+        <v>91</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1083,8 +1227,23 @@
       <c r="C19">
         <v>18.192335</v>
       </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19">
+        <v>56</v>
+      </c>
+      <c r="H19" t="s">
+        <v>91</v>
+      </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1092,13 +1251,28 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-22.615736999999999</v>
+        <v>-22.613410999999999</v>
       </c>
       <c r="C20">
-        <v>18.192335</v>
+        <v>18.193518999999998</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20">
+        <v>45</v>
+      </c>
+      <c r="H20" t="s">
+        <v>92</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1111,8 +1285,23 @@
       <c r="C21">
         <v>18.193518999999998</v>
       </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21">
+        <v>38</v>
+      </c>
+      <c r="H21" t="s">
+        <v>92</v>
+      </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1125,8 +1314,23 @@
       <c r="C22">
         <v>18.193518999999998</v>
       </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>92</v>
+      </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1139,8 +1343,23 @@
       <c r="C23">
         <v>18.193518999999998</v>
       </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>92</v>
+      </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1153,8 +1372,23 @@
       <c r="C24">
         <v>18.193518999999998</v>
       </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24">
+        <v>33</v>
+      </c>
+      <c r="H24" t="s">
+        <v>92</v>
+      </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1167,8 +1401,23 @@
       <c r="C25">
         <v>18.193518999999998</v>
       </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25">
+        <v>64</v>
+      </c>
+      <c r="H25" t="s">
+        <v>92</v>
+      </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1181,8 +1430,23 @@
       <c r="C26">
         <v>18.193518999999998</v>
       </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26">
+        <v>44</v>
+      </c>
+      <c r="H26" t="s">
+        <v>92</v>
+      </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1190,13 +1454,22 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-22.613410999999999</v>
+        <v>-22.683319000000001</v>
       </c>
       <c r="C27">
-        <v>18.193518999999998</v>
+        <v>18.160800999999999</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" t="s">
+        <v>91</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1209,8 +1482,17 @@
       <c r="C28">
         <v>18.160800999999999</v>
       </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" t="s">
+        <v>91</v>
+      </c>
       <c r="I28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1218,13 +1500,22 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-22.683319000000001</v>
+        <v>-22.683382000000002</v>
       </c>
       <c r="C29">
-        <v>18.160800999999999</v>
+        <v>18.16094</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" t="s">
+        <v>81</v>
       </c>
       <c r="I29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -1232,16 +1523,22 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-22.683382000000002</v>
+        <v>-22.683562999999999</v>
       </c>
       <c r="C30">
-        <v>18.16094</v>
+        <v>18.16095</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
       </c>
       <c r="H30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -1254,8 +1551,17 @@
       <c r="C31">
         <v>18.16095</v>
       </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" t="s">
+        <v>81</v>
+      </c>
       <c r="I31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -1263,13 +1569,22 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-22.683562999999999</v>
+        <v>-22.683741999999999</v>
       </c>
       <c r="C32">
-        <v>18.16095</v>
+        <v>18.160822</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" t="s">
+        <v>70</v>
       </c>
       <c r="I32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -1282,8 +1597,17 @@
       <c r="C33">
         <v>18.160822</v>
       </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" t="s">
+        <v>70</v>
+      </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -1291,21 +1615,57 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-22.683741999999999</v>
+        <v>-22.683845999999999</v>
       </c>
       <c r="C34">
-        <v>18.160822</v>
+        <v>18.160353000000001</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34">
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>70</v>
       </c>
       <c r="I34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
+      <c r="B35">
+        <v>-22.683966000000002</v>
+      </c>
+      <c r="C35">
+        <v>18.160235</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35">
+        <v>61</v>
+      </c>
+      <c r="H35" t="s">
+        <v>70</v>
+      </c>
       <c r="I35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -1318,8 +1678,23 @@
       <c r="C36">
         <v>18.160235</v>
       </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36">
+        <v>52</v>
+      </c>
+      <c r="H36" t="s">
+        <v>70</v>
+      </c>
       <c r="I36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -1332,8 +1707,23 @@
       <c r="C37">
         <v>18.160235</v>
       </c>
+      <c r="D37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37">
+        <v>62</v>
+      </c>
+      <c r="H37" t="s">
+        <v>70</v>
+      </c>
       <c r="I37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -1341,13 +1731,28 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>-22.683966000000002</v>
+        <v>-22.683512</v>
       </c>
       <c r="C38">
-        <v>18.160235</v>
+        <v>18.161339000000002</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38">
+        <v>46</v>
+      </c>
+      <c r="H38" t="s">
+        <v>80</v>
       </c>
       <c r="I38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -1360,11 +1765,23 @@
       <c r="C39">
         <v>18.161339000000002</v>
       </c>
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39">
+        <v>59</v>
+      </c>
       <c r="H39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -1377,11 +1794,23 @@
       <c r="C40">
         <v>18.161339000000002</v>
       </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40">
+        <v>56</v>
+      </c>
       <c r="H40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -1394,11 +1823,23 @@
       <c r="C41">
         <v>18.161339000000002</v>
       </c>
+      <c r="D41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41">
+        <v>56</v>
+      </c>
       <c r="H41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -1411,11 +1852,23 @@
       <c r="C42">
         <v>18.161339000000002</v>
       </c>
+      <c r="D42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42">
+        <v>71</v>
+      </c>
       <c r="H42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -1428,11 +1881,23 @@
       <c r="C43">
         <v>18.161339000000002</v>
       </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43">
+        <v>46</v>
+      </c>
       <c r="H43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -1445,11 +1910,20 @@
       <c r="C44">
         <v>18.161339000000002</v>
       </c>
+      <c r="D44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" t="s">
+        <v>62</v>
+      </c>
+      <c r="G44">
+        <v>12</v>
+      </c>
       <c r="H44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -1457,16 +1931,28 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>-22.683512</v>
+        <v>-22.586753000000002</v>
       </c>
       <c r="C45">
-        <v>18.161339000000002</v>
+        <v>18.184711</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45">
+        <v>55</v>
       </c>
       <c r="H45" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="I45" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -1474,13 +1960,28 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>-22.586753000000002</v>
+        <v>-22.583613</v>
       </c>
       <c r="C46">
-        <v>18.184711</v>
+        <v>18.186368999999999</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46">
+        <v>45</v>
+      </c>
+      <c r="H46" t="s">
+        <v>70</v>
       </c>
       <c r="I46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -1493,8 +1994,23 @@
       <c r="C47">
         <v>18.186368999999999</v>
       </c>
+      <c r="D47" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47">
+        <v>63</v>
+      </c>
+      <c r="F47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47">
+        <v>63</v>
+      </c>
+      <c r="H47" t="s">
+        <v>70</v>
+      </c>
       <c r="I47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -1502,13 +2018,28 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>-22.583613</v>
+        <v>-22.582934999999999</v>
       </c>
       <c r="C48">
-        <v>18.186368999999999</v>
+        <v>18.186706000000001</v>
+      </c>
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48">
+        <v>62</v>
+      </c>
+      <c r="H48" t="s">
+        <v>70</v>
       </c>
       <c r="I48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -1516,13 +2047,28 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>-22.582934999999999</v>
+        <v>-22.579135999999998</v>
       </c>
       <c r="C49">
-        <v>18.186706000000001</v>
+        <v>18.194229</v>
+      </c>
+      <c r="D49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49">
+        <v>57</v>
+      </c>
+      <c r="H49" t="s">
+        <v>70</v>
       </c>
       <c r="I49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -1530,13 +2076,28 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>-22.579135999999998</v>
+        <v>-22.579395000000002</v>
       </c>
       <c r="C50">
-        <v>18.194229</v>
+        <v>18.192067000000002</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50">
+        <v>36</v>
+      </c>
+      <c r="H50" t="s">
+        <v>70</v>
       </c>
       <c r="I50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -1544,13 +2105,28 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>-22.579395000000002</v>
+        <v>-22.579473</v>
       </c>
       <c r="C51">
-        <v>18.192067000000002</v>
+        <v>18.191019000000001</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" t="s">
+        <v>87</v>
+      </c>
+      <c r="F51" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51">
+        <v>40</v>
+      </c>
+      <c r="H51" t="s">
+        <v>70</v>
       </c>
       <c r="I51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -1563,8 +2139,23 @@
       <c r="C52">
         <v>18.191019000000001</v>
       </c>
+      <c r="D52" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" t="s">
+        <v>63</v>
+      </c>
+      <c r="G52">
+        <v>28</v>
+      </c>
+      <c r="H52" t="s">
+        <v>70</v>
+      </c>
       <c r="I52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -1572,13 +2163,28 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>-22.579473</v>
+        <v>-22.579015999999999</v>
       </c>
       <c r="C53">
-        <v>18.191019000000001</v>
+        <v>18.190398999999999</v>
+      </c>
+      <c r="D53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" t="s">
+        <v>63</v>
+      </c>
+      <c r="G53">
+        <v>39</v>
+      </c>
+      <c r="H53" t="s">
+        <v>70</v>
       </c>
       <c r="I53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -1586,13 +2192,28 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>-22.579015999999999</v>
+        <v>-22.577597000000001</v>
       </c>
       <c r="C54">
-        <v>18.190398999999999</v>
+        <v>18.191299000000001</v>
+      </c>
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F54" t="s">
+        <v>63</v>
+      </c>
+      <c r="G54">
+        <v>79</v>
+      </c>
+      <c r="H54" t="s">
+        <v>70</v>
       </c>
       <c r="I54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -1600,13 +2221,28 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>-22.577597000000001</v>
+        <v>-22.577245999999999</v>
       </c>
       <c r="C55">
-        <v>18.191299000000001</v>
+        <v>18.191355999999999</v>
+      </c>
+      <c r="D55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" t="s">
+        <v>87</v>
+      </c>
+      <c r="F55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G55">
+        <v>51</v>
+      </c>
+      <c r="H55" t="s">
+        <v>70</v>
       </c>
       <c r="I55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -1614,31 +2250,30 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>-22.577245999999999</v>
+        <v>-22.575707999999999</v>
       </c>
       <c r="C56">
-        <v>18.191355999999999</v>
+        <v>18.191939999999999</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="F56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G56">
+        <v>49</v>
+      </c>
+      <c r="H56" t="s">
+        <v>70</v>
       </c>
       <c r="I56" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57">
-        <v>-22.575707999999999</v>
-      </c>
-      <c r="C57">
-        <v>18.191939999999999</v>
-      </c>
-      <c r="I57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>